<commit_message>
Permissions zapped, now should all be based on the home menu for normal and master users
git-svn-id: http://192.168.1.10/repos/toto@2131 b53939d4-f08c-4181-96d4-b201aa9c61c4
</commit_message>
<xml_diff>
--- a/Toto/trunk/web/WEB-INF/AzquoUsers.xlsx
+++ b/Toto/trunk/web/WEB-INF/AzquoUsers.xlsx
@@ -5,17 +5,22 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -24,6 +29,21 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>Report</t>
   </si>
 </sst>
 </file>
@@ -154,7 +174,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -187,18 +207,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.6734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.68367346938776"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -208,11 +228,23 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -220,7 +252,7 @@
       <c r="E2" s="5"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -228,7 +260,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -236,7 +268,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -244,7 +276,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -252,7 +284,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -260,7 +292,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -268,7 +300,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>

</xml_diff>

<commit_message>
Smartly formatted.  Dates on AzquoUser formatted as text
git-svn-id: http://192.168.1.10/repos/toto@2168 b53939d4-f08c-4181-96d4-b201aa9c61c4
</commit_message>
<xml_diff>
--- a/Toto/trunk/web/WEB-INF/AzquoUsers.xlsx
+++ b/Toto/trunk/web/WEB-INF/AzquoUsers.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bill\projects\Toto\web\WEB-INF\"/>
@@ -14,8 +14,11 @@
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <definedNames>
-    <definedName name="az_Business">Users!$E$2</definedName>
+    <definedName name="az_Business">Users!$B$3</definedName>
     <definedName name="az_ListStart">Users!$A$6</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -33,12 +36,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>End Date</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>Database</t>
   </si>
   <si>
@@ -52,13 +49,19 @@
   </si>
   <si>
     <t xml:space="preserve">List of users for </t>
+  </si>
+  <si>
+    <t>End Date - please write yyyy-mm-dd</t>
+  </si>
+  <si>
+    <t>Status - Administrator, Developer, Master, User</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -93,13 +96,25 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="53"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -114,17 +129,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -147,39 +175,33 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>76201</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>133351</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1649405</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>548269</xdr:rowOff>
+      <xdr:rowOff>647701</xdr:rowOff>
     </xdr:to>
-    <xdr:pic>
+    <xdr:pic macro="[1]!ClearAll">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="4" name="Picture 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="19050"/>
-          <a:ext cx="1400175" cy="529219"/>
+          <a:off x="76201" y="133351"/>
+          <a:ext cx="1573204" cy="514350"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -189,6 +211,26 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Analysis"/>
+      <sheetName val="Template"/>
+      <sheetName val="Azquo constants"/>
+    </sheetNames>
+    <definedNames>
+      <definedName name="ClearAll"/>
+    </definedNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -488,120 +530,129 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="6" width="19.28515625" style="1" customWidth="1"/>
-    <col min="7" max="1024" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="30.140625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="19.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="39.85546875" style="1" customWidth="1"/>
+    <col min="8" max="1024" width="8.7109375" style="1"/>
     <col min="1025" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="C2" s="6" t="s">
+    <row r="1" spans="1:7" s="6" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="8"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="3" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5"/>
+    </row>
+    <row r="5" spans="1:7" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>